<commit_message>
more login and template pages and test
</commit_message>
<xml_diff>
--- a/Decidim_Automated_Testing/Configuration/DecidimLoginData.xlsx
+++ b/Decidim_Automated_Testing/Configuration/DecidimLoginData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="435" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="435" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Full2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>Decidim User Login</t>
   </si>
@@ -48,6 +49,18 @@
   </si>
   <si>
     <t>password5</t>
+  </si>
+  <si>
+    <t>decidim</t>
+  </si>
+  <si>
+    <t>ADMIN@example.org</t>
+  </si>
+  <si>
+    <t>USER@example.org</t>
+  </si>
+  <si>
+    <t>INJECTED CODE</t>
   </si>
 </sst>
 </file>
@@ -157,8 +170,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -232,4 +245,168 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Pàgina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="admin@example.org"/>
+    <hyperlink ref="A3" r:id="rId2" display="user@example.org"/>
+    <hyperlink ref="A7" r:id="rId3" display="ADMIN@example.org"/>
+    <hyperlink ref="A8" r:id="rId4" display="USER@example.org"/>
+    <hyperlink ref="A9" r:id="rId5" display="admin@example.org"/>
+    <hyperlink ref="A10" r:id="rId6" display="user@example.org"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Pàgina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>